<commit_message>
fix bash for test003
</commit_message>
<xml_diff>
--- a/execution time.xlsx
+++ b/execution time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://endava-my.sharepoint.com/personal/alexandr_binkovski_endava_com/Documents/Documents/SelfDevelopment/AI/Whisper/OpenAIWhisper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_F25DC773A252ABDACC10486951184EDA5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B50BE82A-16CE-491A-B9DF-547B7BD97310}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_F25DC773A252ABDACC10486951184EDA5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C0DE133-4C32-461D-B0B3-002985CD562F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Model</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>test002 - RU with translation</t>
+  </si>
+  <si>
+    <t>test003 - RO</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -181,24 +184,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,31 +260,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Processing per second comparison</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -397,7 +401,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9046-4E83-8E64-BF4D30E2C192}"/>
+              <c16:uniqueId val="{00000001-EE6F-4ABE-A526-B21AFD0313E2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -507,7 +511,117 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9046-4E83-8E64-BF4D30E2C192}"/>
+              <c16:uniqueId val="{00000003-EE6F-4ABE-A526-B21AFD0313E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CPU based - test results'!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Input dataset</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test003 - RO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Processing per Sec.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CPU based - test results'!$A$4:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>tiny</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>small</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>medium</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>large</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>large-v2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>large-v3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CPU based - test results'!$G$4:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.2146560132816652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EE6F-4ABE-A526-B21AFD0313E2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -521,8 +635,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1516134223"/>
-        <c:axId val="1264553551"/>
+        <c:axId val="702996047"/>
+        <c:axId val="308366543"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -650,7 +764,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-9046-4E83-8E64-BF4D30E2C192}"/>
+                    <c16:uniqueId val="{00000000-EE6F-4ABE-A526-B21AFD0313E2}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -780,7 +894,119 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-9046-4E83-8E64-BF4D30E2C192}"/>
+                    <c16:uniqueId val="{00000002-EE6F-4ABE-A526-B21AFD0313E2}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'CPU based - test results'!$F$1:$F$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>Input dataset</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>test003 - RO</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Processing time (sec.)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'CPU based - test results'!$A$4:$A$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>tiny</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>base</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>small</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>medium</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>large</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>large-v2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>large-v3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'CPU based - test results'!$F$4:$F$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>4846.9327799000002</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-EE6F-4ABE-A526-B21AFD0313E2}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -789,7 +1015,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1516134223"/>
+        <c:axId val="702996047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +1058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1264553551"/>
+        <c:crossAx val="308366543"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -840,7 +1066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1264553551"/>
+        <c:axId val="308366543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +1117,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1516134223"/>
+        <c:crossAx val="702996047"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1525,23 +1751,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1FCE641-4691-F96F-14C2-E366D2415129}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E85CB942-A1DA-EF65-30FB-F8A72C0AEF85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1920,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1933,32 +2159,40 @@
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1971,8 +2205,14 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1983,15 +2223,22 @@
         <f>B4/18</f>
         <v>0.49224061111111111</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>48.515885900000001</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <f>D4/57</f>
         <v>0.8511558929824562</v>
       </c>
+      <c r="F4" s="4">
+        <v>4846.9327799000002</v>
+      </c>
+      <c r="G4" s="4">
+        <f>F4/22580</f>
+        <v>0.2146560132816652</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1999,18 +2246,23 @@
         <v>12.335821899999999</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:E10" si="0">B5/18</f>
+        <f t="shared" ref="C5:C10" si="0">B5/18</f>
         <v>0.6853234388888888</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>54.678554300000002</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <f t="shared" ref="E5:E10" si="1">D5/57</f>
         <v>0.9592728824561404</v>
       </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G10" si="2">F5/22580</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2028,8 +2280,13 @@
         <f t="shared" si="1"/>
         <v>1.5925737350877194</v>
       </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2047,8 +2304,13 @@
         <f t="shared" si="1"/>
         <v>4.7740344578947367</v>
       </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2066,8 +2328,13 @@
         <f t="shared" si="1"/>
         <v>8.2033155087719294</v>
       </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2085,8 +2352,13 @@
         <f t="shared" si="1"/>
         <v>8.8147719684210522</v>
       </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2104,13 +2376,19 @@
         <f t="shared" si="1"/>
         <v>8.4154917701754393</v>
       </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix diactitics on persistence. Recalculate models to be on the same processor performance
</commit_message>
<xml_diff>
--- a/execution time.xlsx
+++ b/execution time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://endava-my.sharepoint.com/personal/alexandr_binkovski_endava_com/Documents/Documents/SelfDevelopment/AI/Whisper/OpenAIWhisper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="11_F25DC773A252ABDACC10486951184EDA5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C0DE133-4C32-461D-B0B3-002985CD562F}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="11_F25DC773A252ABDACC10486951184EDA5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F1B595-406D-4D7C-95B3-DE272D200B49}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Model</t>
   </si>
@@ -120,10 +120,13 @@
     <t>test001 - EN</t>
   </si>
   <si>
-    <t>test002 - RU with translation</t>
-  </si>
-  <si>
     <t>test003 - RO</t>
+  </si>
+  <si>
+    <t>test002 - RU</t>
+  </si>
+  <si>
+    <t>test002 - RU - Translate to EN</t>
   </si>
 </sst>
 </file>
@@ -375,25 +378,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.49224061111111111</c:v>
+                  <c:v>0.53647939999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6853234388888888</c:v>
+                  <c:v>0.70843614444444436</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5547813611111112</c:v>
+                  <c:v>1.7056488944444446</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8464272777777779</c:v>
+                  <c:v>5.1646559777777776</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.074200205555556</c:v>
+                  <c:v>9.8011601611111114</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4773714555555557</c:v>
+                  <c:v>9.5391842944444445</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.682097938888889</c:v>
+                  <c:v>9.0973455722222223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,7 +404,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EE6F-4ABE-A526-B21AFD0313E2}"/>
+              <c16:uniqueId val="{00000001-8B36-4AB7-8181-95251C2A79AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -417,7 +420,7 @@
                   <c:v>Input dataset</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>test002 - RU with translation</c:v>
+                  <c:v>test002 - RU - Translate to EN</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Processing per Sec.</c:v>
@@ -485,25 +488,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.8511558929824562</c:v>
+                  <c:v>0.91508839298245614</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9592728824561404</c:v>
+                  <c:v>1.0539678140350877</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5925737350877194</c:v>
+                  <c:v>1.6745025263157896</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.7740344578947367</c:v>
+                  <c:v>5.2263322789473685</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.2033155087719294</c:v>
+                  <c:v>8.8656462736842112</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.8147719684210522</c:v>
+                  <c:v>9.1548743105263171</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4154917701754393</c:v>
+                  <c:v>8.8585294473684204</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -511,7 +514,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-EE6F-4ABE-A526-B21AFD0313E2}"/>
+              <c16:uniqueId val="{00000003-8B36-4AB7-8181-95251C2A79AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -527,7 +530,7 @@
                   <c:v>Input dataset</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>test003 - RO</c:v>
+                  <c:v>test002 - RU</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Processing per Sec.</c:v>
@@ -595,25 +598,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.2146560132816652</c:v>
+                  <c:v>0.36058116315789474</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.62624022280701763</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.8705372894736843</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5.6404988736842103</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>10.817850142105264</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9.9414686894736857</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>11.053002324561405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -621,7 +624,123 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-EE6F-4ABE-A526-B21AFD0313E2}"/>
+              <c16:uniqueId val="{00000005-8B36-4AB7-8181-95251C2A79AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CPU based - test results'!$I$1:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Input dataset</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test003 - RO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Processing per Sec.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CPU based - test results'!$A$4:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>tiny</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>small</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>medium</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>large</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>large-v2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>large-v3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CPU based - test results'!$I$4:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.2146560132816652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-8B36-4AB7-8181-95251C2A79AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -635,8 +754,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="702996047"/>
-        <c:axId val="308366543"/>
+        <c:axId val="1457262191"/>
+        <c:axId val="946532207"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -738,25 +857,25 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>8.8603310000000004</c:v>
+                        <c:v>9.6566291999999994</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>12.335821899999999</c:v>
+                        <c:v>12.751850599999999</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>27.986064500000001</c:v>
+                        <c:v>30.701680100000001</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>87.235691000000003</c:v>
+                        <c:v>92.963807599999996</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>163.33560370000001</c:v>
+                        <c:v>176.42088290000001</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>152.5926862</c:v>
+                        <c:v>171.70531729999999</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>156.2777629</c:v>
+                        <c:v>163.7522203</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -764,7 +883,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-EE6F-4ABE-A526-B21AFD0313E2}"/>
+                    <c16:uniqueId val="{00000000-8B36-4AB7-8181-95251C2A79AC}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -788,7 +907,7 @@
                         <c:v>Input dataset</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>test002 - RU with translation</c:v>
+                        <c:v>test002 - RU - Translate to EN</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>Processing time (sec.)</c:v>
@@ -868,25 +987,25 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>48.515885900000001</c:v>
+                        <c:v>52.160038399999998</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>54.678554300000002</c:v>
+                        <c:v>60.076165400000001</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>90.776702900000004</c:v>
+                        <c:v>95.446644000000006</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>272.1199641</c:v>
+                        <c:v>297.90093990000003</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>467.58898399999998</c:v>
+                        <c:v>505.34183760000002</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>502.44200219999999</c:v>
+                        <c:v>521.82783570000004</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>479.68303090000001</c:v>
+                        <c:v>504.93617849999998</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -894,7 +1013,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-EE6F-4ABE-A526-B21AFD0313E2}"/>
+                    <c16:uniqueId val="{00000002-8B36-4AB7-8181-95251C2A79AC}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -918,7 +1037,7 @@
                         <c:v>Input dataset</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>test003 - RO</c:v>
+                        <c:v>test002 - RU</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>Processing time (sec.)</c:v>
@@ -998,7 +1117,25 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>4846.9327799000002</c:v>
+                        <c:v>20.553126299999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>35.695692700000002</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>106.6206255</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>321.50843579999997</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>616.61745810000002</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>566.66371530000004</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>630.02113250000002</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1006,7 +1143,125 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-EE6F-4ABE-A526-B21AFD0313E2}"/>
+                    <c16:uniqueId val="{00000004-8B36-4AB7-8181-95251C2A79AC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="6"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'CPU based - test results'!$H$1:$H$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>Input dataset</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>test003 - RO</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Processing time (sec.)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'CPU based - test results'!$A$4:$A$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>tiny</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>base</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>small</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>medium</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>large</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>large-v2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>large-v3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'CPU based - test results'!$H$4:$H$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>4846.9327799000002</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-8B36-4AB7-8181-95251C2A79AC}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1015,7 +1270,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="702996047"/>
+        <c:axId val="1457262191"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,7 +1313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308366543"/>
+        <c:crossAx val="946532207"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1066,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="308366543"/>
+        <c:axId val="946532207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1117,7 +1372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="702996047"/>
+        <c:crossAx val="1457262191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1751,23 +2006,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E85CB942-A1DA-EF65-30FB-F8A72C0AEF85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE8CEF69-CCD0-AC25-A711-2547DE6BBDAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2146,10 +2401,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2159,11 +2414,12 @@
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2175,23 +2431,29 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -2211,184 +2473,240 @@
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>8.8603310000000004</v>
+        <v>9.6566291999999994</v>
       </c>
       <c r="C4" s="1">
         <f>B4/18</f>
-        <v>0.49224061111111111</v>
+        <v>0.53647939999999994</v>
       </c>
       <c r="D4" s="4">
-        <v>48.515885900000001</v>
+        <v>52.160038399999998</v>
       </c>
       <c r="E4" s="4">
         <f>D4/57</f>
-        <v>0.8511558929824562</v>
+        <v>0.91508839298245614</v>
       </c>
       <c r="F4" s="4">
+        <v>20.553126299999999</v>
+      </c>
+      <c r="G4" s="4">
+        <f>F4/57</f>
+        <v>0.36058116315789474</v>
+      </c>
+      <c r="H4" s="4">
         <v>4846.9327799000002</v>
       </c>
-      <c r="G4" s="4">
-        <f>F4/22580</f>
+      <c r="I4" s="4">
+        <f>H4/22580</f>
         <v>0.2146560132816652</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>12.335821899999999</v>
+        <v>12.751850599999999</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ref="C5:C10" si="0">B5/18</f>
-        <v>0.6853234388888888</v>
+        <v>0.70843614444444436</v>
       </c>
       <c r="D5" s="4">
-        <v>54.678554300000002</v>
+        <v>60.076165400000001</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" ref="E5:E10" si="1">D5/57</f>
-        <v>0.9592728824561404</v>
-      </c>
-      <c r="F5" s="4"/>
+        <v>1.0539678140350877</v>
+      </c>
+      <c r="F5" s="4">
+        <v>35.695692700000002</v>
+      </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G10" si="2">F5/22580</f>
+        <f t="shared" ref="G5:G10" si="2">F5/57</f>
+        <v>0.62624022280701763</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4">
+        <f t="shared" ref="I5:I10" si="3">H5/22580</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>27.986064500000001</v>
+        <v>30.701680100000001</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>1.5547813611111112</v>
+        <v>1.7056488944444446</v>
       </c>
       <c r="D6" s="1">
-        <v>90.776702900000004</v>
+        <v>95.446644000000006</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>1.5925737350877194</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>1.6745025263157896</v>
+      </c>
+      <c r="F6" s="1">
+        <v>106.6206255</v>
+      </c>
       <c r="G6" s="4">
         <f t="shared" si="2"/>
+        <v>1.8705372894736843</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>87.235691000000003</v>
+        <v>92.963807599999996</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>4.8464272777777779</v>
+        <v>5.1646559777777776</v>
       </c>
       <c r="D7" s="1">
-        <v>272.1199641</v>
+        <v>297.90093990000003</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>4.7740344578947367</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>5.2263322789473685</v>
+      </c>
+      <c r="F7" s="1">
+        <v>321.50843579999997</v>
+      </c>
       <c r="G7" s="4">
         <f t="shared" si="2"/>
+        <v>5.6404988736842103</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>163.33560370000001</v>
+        <v>176.42088290000001</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>9.074200205555556</v>
+        <v>9.8011601611111114</v>
       </c>
       <c r="D8" s="1">
-        <v>467.58898399999998</v>
+        <v>505.34183760000002</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
-        <v>8.2033155087719294</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>8.8656462736842112</v>
+      </c>
+      <c r="F8" s="1">
+        <v>616.61745810000002</v>
+      </c>
       <c r="G8" s="4">
         <f t="shared" si="2"/>
+        <v>10.817850142105264</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>152.5926862</v>
+        <v>171.70531729999999</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>8.4773714555555557</v>
+        <v>9.5391842944444445</v>
       </c>
       <c r="D9" s="1">
-        <v>502.44200219999999</v>
+        <v>521.82783570000004</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="1"/>
-        <v>8.8147719684210522</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>9.1548743105263171</v>
+      </c>
+      <c r="F9" s="1">
+        <v>566.66371530000004</v>
+      </c>
       <c r="G9" s="4">
         <f t="shared" si="2"/>
+        <v>9.9414686894736857</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>156.2777629</v>
+        <v>163.7522203</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>8.682097938888889</v>
+        <v>9.0973455722222223</v>
       </c>
       <c r="D10" s="1">
-        <v>479.68303090000001</v>
+        <v>504.93617849999998</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>8.4154917701754393</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>8.8585294473684204</v>
+      </c>
+      <c r="F10" s="1">
+        <v>630.02113250000002</v>
+      </c>
       <c r="G10" s="4">
         <f t="shared" si="2"/>
+        <v>11.053002324561405</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="4">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A1:A3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B1:I1"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>